<commit_message>
Medium Import Size Performance Enhanced
</commit_message>
<xml_diff>
--- a/public/templates/ImporAkunSiswa.xlsx
+++ b/public/templates/ImporAkunSiswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Project\Laravel\AgendaKBM\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066CB02D-2CEE-4D96-8000-8FC471DAEB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7FD7E5-CE36-4491-AA45-41A9FF67AE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C244CCC3-0CB0-4766-944C-65F558DCEF66}"/>
   </bookViews>
@@ -36,53 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
     <t>EMAIL</t>
   </si>
   <si>
     <t>PASSWORD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">INSTRUKSI
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Username Minimal 5 Karakter
-Username Maksimal 25 Karakter
-Username Tidak Boleh Sama</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mulai Mengisi Pada Baris 3 Dibawah</t>
-    </r>
   </si>
   <si>
     <r>
@@ -121,46 +78,6 @@
       </rPr>
       <t>Buat Password Yang Kuat!
 Mulai Mengisi Pada Baris 3 Dibawah</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">INSTRUKSI
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Email Maksimal 255 Karakter
-Email Tidak Boleh Sama
-Merupakan Email Valid Yang Aktif</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mulai Mengisi Pada Baris 3 Dibawah</t>
     </r>
   </si>
   <si>
@@ -266,6 +183,88 @@
       <t>Sesuaikan Penulisan Kelas Dengan
 Data Yang Ada Di Aplikasi Agenda
 (Contoh : XII RPL 1)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mulai Mengisi Pada Baris 3 Dibawah</t>
+    </r>
+  </si>
+  <si>
+    <t>NIS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INSTRUKSI
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Merupakan Email Valid Yang Aktif
+Kosongkan Jika Tidak Memiliki Data Email</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mulai Mengisi Pada Baris 3 Dibawah</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INSTRUKSI
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NIS Siswa Maksimal 10 Karakter
+NIS Siswa Minimal 9 Karakter
+NIS Tidak Boleh Sama</t>
     </r>
     <r>
       <rPr>
@@ -295,7 +294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +314,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -671,14 +676,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3:F1233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="36.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+    <col min="2" max="3" width="35.77734375" customWidth="1"/>
     <col min="4" max="4" width="36.88671875" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="22.44140625" customWidth="1"/>
@@ -686,45 +690,46 @@
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>